<commit_message>
v1 done, to be deploy
to be deploy
</commit_message>
<xml_diff>
--- a/donefiles/test.xlsx
+++ b/donefiles/test.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -359,12 +359,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve">	数据工程师</t>
+          <t>数据工程师</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t xml:space="preserve">	算法工程师</t>
+          <t>算法工程师</t>
         </is>
       </c>
       <c r="D1" t="n">
@@ -377,12 +377,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">	数据挖掘工程师</t>
+          <t>数据挖掘工程师</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">	数据挖掘</t>
+          <t>数据挖掘</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -395,12 +395,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">	大数据开发工程师</t>
+          <t>大数据开发工程师</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">	算法工程师</t>
+          <t>算法工程师</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -413,12 +413,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">	机器学习工程师</t>
+          <t>机器学习工程师</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">	算法工程师</t>
+          <t>算法工程师</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -431,34 +431,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">	数据科学家</t>
+          <t>数据科学家</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">	数据挖掘</t>
+          <t>数据挖掘</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>44</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">		</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">		</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>